<commit_message>
Poprawna obsługa dyscyplin HST (#1331)
</commit_message>
<xml_diff>
--- a/src/import_dyscyplin/tests/test5_kasowanie_subdyscypliny.xlsx
+++ b/src/import_dyscyplin/tests/test5_kasowanie_subdyscypliny.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpasternak/Programowanie/bpp/src/import_dyscyplin/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BD833D-EB0E-AA4A-86C4-CC300022D024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE47D50-3448-2F42-AC75-700162031CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28520" windowHeight="12000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -139,7 +139,7 @@
     <t>memetyka stosowana</t>
   </si>
   <si>
-    <t>1.1</t>
+    <t>3.1</t>
   </si>
 </sst>
 </file>
@@ -327,62 +327,62 @@
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -669,7 +669,7 @@
   <dimension ref="A1:K1341"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>